<commit_message>
Apply reduced leakage rate on methyl chloride emissions from trimethylchlorosilane production.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-LiS.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-LiS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB01BC2-6BC6-0240-9BB6-29B928A36F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA59D2-4254-5241-BA6C-F264677CD2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31560" yWindow="-860" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - Li-S" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3165" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="464">
   <si>
     <t>Activity</t>
   </si>
@@ -1433,9 +1433,6 @@
     <t>this is LiTFSI. Source: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141</t>
   </si>
   <si>
-    <t>This is a multi-output process. As openLCA (which I used in this study) can handle this kind of processes, I have not done any allocation in the dataset, but instead used the allocation-function in OpenLCA. This dataset is mass-allocated to the product "trimethylchlorosilane" (3%w/w) in the study. Source: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141</t>
-  </si>
-  <si>
     <t>Specific energy density: 150 Wh/kg. Projected up to 500 Wh/kg in an optimistic future || Cycle life: 1500 || Lifetime: 225 kWh/kg.Source: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141</t>
   </si>
   <si>
@@ -1569,6 +1566,24 @@
   </si>
   <si>
     <t>battery, Li-S</t>
+  </si>
+  <si>
+    <t>This is a multi-output process, which produces dimethylchlorosilane (97%) but also trimethylchlorosilane (3%). The ecoinvent dataset for trimethylchlorosilane has been re-allocated to produce a proxy for dimethylchlorosilane production, based on a mass allocation. Note that, compared to the oroginal values in ecoinvent and also Wickerts et al., 2023, we have reduced the emission of methyl chloride, a potent ozone-depleting gas, to 1%, instead of 4.5%, which seems to ignore current efforts in limiting venting of such gases and promoting recovery instead. According to this report (https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf), the current leak rate in the EU is about 0.06%. Source: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141</t>
+  </si>
+  <si>
+    <t>Original value in Wickerts et al., 2023 of 0.0412, representing a 4.5% leakage rate. This was reduced to 1% leakage rate. According to https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf, current leakage rate in the EU is 0.06%.</t>
+  </si>
+  <si>
+    <t>uncertainty type</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1760,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1775,6 +1790,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2059,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1076"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D465" sqref="D465"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2901,13 +2917,13 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B64" s="8"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B65" s="8"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -2915,15 +2931,15 @@
         <v>324</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="10" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="29" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -2931,7 +2947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2939,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2947,7 +2963,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2955,7 +2971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2963,12 +2979,12 @@
         <v>296</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -2993,8 +3009,20 @@
       <c r="H75" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>460</v>
+      </c>
+      <c r="J75" t="s">
+        <v>461</v>
+      </c>
+      <c r="K75" t="s">
+        <v>462</v>
+      </c>
+      <c r="L75" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>324</v>
       </c>
@@ -3014,7 +3042,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -3035,10 +3063,10 @@
         <v>39</v>
       </c>
       <c r="H77" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -3059,7 +3087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>267</v>
       </c>
@@ -3080,7 +3108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>268</v>
       </c>
@@ -3101,7 +3129,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>268</v>
       </c>
@@ -3122,7 +3150,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>270</v>
       </c>
@@ -3143,7 +3171,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>270</v>
       </c>
@@ -3164,7 +3192,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>68</v>
       </c>
@@ -3185,7 +3213,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -3206,7 +3234,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>272</v>
       </c>
@@ -3227,7 +3255,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>274</v>
       </c>
@@ -3248,7 +3276,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>398</v>
       </c>
@@ -3266,7 +3294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>399</v>
       </c>
@@ -3284,7 +3312,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>402</v>
       </c>
@@ -3302,7 +3330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>49</v>
       </c>
@@ -3323,7 +3351,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>49</v>
       </c>
@@ -3344,7 +3372,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>49</v>
       </c>
@@ -3365,7 +3393,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>401</v>
       </c>
@@ -3383,13 +3411,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>400</v>
       </c>
       <c r="B95" s="13">
-        <f>0.0413</f>
-        <v>4.1300000000000003E-2</v>
+        <f>0.01*SUM(B82:B83)</f>
+        <v>8.2594999999999995E-3</v>
       </c>
       <c r="C95" t="s">
         <v>7</v>
@@ -3400,8 +3428,25 @@
       <c r="F95" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>459</v>
+      </c>
+      <c r="I95">
+        <v>5</v>
+      </c>
+      <c r="J95" s="13">
+        <f>B95</f>
+        <v>8.2594999999999995E-3</v>
+      </c>
+      <c r="K95">
+        <f>0.006*SUM(B82:B83)</f>
+        <v>4.9556999999999995E-3</v>
+      </c>
+      <c r="L95">
+        <v>4.1300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>403</v>
       </c>
@@ -4287,7 +4332,7 @@
         <v>50</v>
       </c>
       <c r="G163" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -4547,7 +4592,7 @@
         <v>50</v>
       </c>
       <c r="H183" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -5346,7 +5391,7 @@
         <v>55</v>
       </c>
       <c r="G245" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.2">
@@ -7398,7 +7443,7 @@
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A404" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B404" s="15">
         <v>0.33</v>
@@ -7414,7 +7459,7 @@
         <v>15</v>
       </c>
       <c r="G404" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.2">
@@ -7911,7 +7956,7 @@
         <v>0</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="440" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -7919,7 +7964,7 @@
         <v>1</v>
       </c>
       <c r="B440" s="26" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="441" spans="1:8" x14ac:dyDescent="0.2">
@@ -7943,7 +7988,7 @@
         <v>5</v>
       </c>
       <c r="B443" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="444" spans="1:8" x14ac:dyDescent="0.2">
@@ -7995,7 +8040,7 @@
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B448">
         <v>1</v>
@@ -8010,7 +8055,7 @@
         <v>13</v>
       </c>
       <c r="G448" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="449" spans="1:8" x14ac:dyDescent="0.2">
@@ -8258,7 +8303,7 @@
         <v>0</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.2">
@@ -8266,7 +8311,7 @@
         <v>1</v>
       </c>
       <c r="B461" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H461" s="5"/>
     </row>
@@ -8307,7 +8352,7 @@
         <v>8</v>
       </c>
       <c r="B466" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.2">
@@ -8340,7 +8385,7 @@
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B469">
         <v>1</v>
@@ -8360,7 +8405,7 @@
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B470">
         <v>1</v>
@@ -8375,7 +8420,7 @@
         <v>15</v>
       </c>
       <c r="F470" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.2">
@@ -8399,7 +8444,7 @@
         <v>24</v>
       </c>
       <c r="G471" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="472" spans="1:7" x14ac:dyDescent="0.2">
@@ -8423,7 +8468,7 @@
         <v>133</v>
       </c>
       <c r="G472" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.2">
@@ -8658,7 +8703,7 @@
         <v>1</v>
       </c>
       <c r="B491" s="16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.2">
@@ -8682,7 +8727,7 @@
         <v>5</v>
       </c>
       <c r="B494" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.2">
@@ -8749,12 +8794,12 @@
         <v>13</v>
       </c>
       <c r="G499" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="500" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B500" s="5">
         <f>408*0.046/24.971</f>
@@ -8773,7 +8818,7 @@
         <v>407</v>
       </c>
       <c r="H500" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="501" spans="1:11" x14ac:dyDescent="0.2">
@@ -8934,7 +8979,7 @@
         <v>0</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="510" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -8942,7 +8987,7 @@
         <v>1</v>
       </c>
       <c r="B510" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.2">
@@ -8966,7 +9011,7 @@
         <v>5</v>
       </c>
       <c r="B513" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="514" spans="1:8" x14ac:dyDescent="0.2">
@@ -8982,7 +9027,7 @@
         <v>8</v>
       </c>
       <c r="B515" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.2">
@@ -9045,7 +9090,7 @@
         <v>battery, Li-S</v>
       </c>
       <c r="H518" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="519" spans="1:8" x14ac:dyDescent="0.2">
@@ -9065,38 +9110,38 @@
         <v>15</v>
       </c>
       <c r="G519" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="520" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B520">
         <v>0.30910727700000001</v>
       </c>
       <c r="C520" t="s">
+        <v>448</v>
+      </c>
+      <c r="E520" t="s">
+        <v>3</v>
+      </c>
+      <c r="F520" t="s">
+        <v>15</v>
+      </c>
+      <c r="G520" t="s">
         <v>449</v>
-      </c>
-      <c r="E520" t="s">
-        <v>3</v>
-      </c>
-      <c r="F520" t="s">
-        <v>15</v>
-      </c>
-      <c r="G520" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="521" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B521">
         <v>2.4627409999999999E-2</v>
       </c>
       <c r="C521" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E521" t="s">
         <v>3</v>
@@ -9105,18 +9150,18 @@
         <v>15</v>
       </c>
       <c r="G521" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="522" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B522">
         <v>0.20877976500000001</v>
       </c>
       <c r="C522" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E522" t="s">
         <v>3</v>
@@ -9125,18 +9170,18 @@
         <v>15</v>
       </c>
       <c r="G522" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="523" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B523">
         <v>0.59901584900000004</v>
       </c>
       <c r="C523" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E523" t="s">
         <v>3</v>
@@ -9145,7 +9190,7 @@
         <v>15</v>
       </c>
       <c r="G523" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="524" spans="1:8" x14ac:dyDescent="0.2">
@@ -12388,10 +12433,10 @@
         <v>15</v>
       </c>
       <c r="F759" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G759" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="760" spans="1:7" x14ac:dyDescent="0.2">
@@ -12962,10 +13007,10 @@
         <v>15</v>
       </c>
       <c r="F811" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G811" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="812" spans="1:7" x14ac:dyDescent="0.2">
@@ -13200,7 +13245,7 @@
         <v>24</v>
       </c>
       <c r="G830" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="831" spans="1:7" x14ac:dyDescent="0.2">
@@ -13224,7 +13269,7 @@
         <v>243</v>
       </c>
       <c r="G831" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="834" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -13649,7 +13694,7 @@
         <v>243</v>
       </c>
       <c r="H874" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="875" spans="1:8" x14ac:dyDescent="0.2">
@@ -13674,7 +13719,7 @@
     </row>
     <row r="876" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A876" s="22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B876">
         <v>-9000</v>
@@ -13689,7 +13734,7 @@
         <v>15</v>
       </c>
       <c r="G876" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="879" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13799,7 +13844,7 @@
         <v>244</v>
       </c>
       <c r="H888" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="889" spans="1:8" x14ac:dyDescent="0.2">
@@ -13819,12 +13864,12 @@
         <v>15</v>
       </c>
       <c r="G889" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="890" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A890" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B890">
         <v>-6.27</v>
@@ -13839,7 +13884,7 @@
         <v>15</v>
       </c>
       <c r="G890" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="894" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13879,7 +13924,7 @@
         <v>5</v>
       </c>
       <c r="B898" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="899" spans="1:8" x14ac:dyDescent="0.2">
@@ -13947,7 +13992,7 @@
         <v>13</v>
       </c>
       <c r="G903" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H903" s="15"/>
     </row>
@@ -13971,7 +14016,7 @@
         <v>249</v>
       </c>
       <c r="H904" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="905" spans="1:8" x14ac:dyDescent="0.2">
@@ -14138,7 +14183,7 @@
         <v>97</v>
       </c>
       <c r="H920" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="921" spans="1:8" x14ac:dyDescent="0.2">
@@ -14203,7 +14248,7 @@
     </row>
     <row r="924" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A924" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B924">
         <v>-4.7E-2</v>
@@ -14218,7 +14263,7 @@
         <v>15</v>
       </c>
       <c r="G924" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="926" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -14328,7 +14373,7 @@
         <v>97</v>
       </c>
       <c r="H935" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="936" spans="1:8" x14ac:dyDescent="0.2">
@@ -14560,7 +14605,7 @@
         <v>0</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="951" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -14592,7 +14637,7 @@
         <v>5</v>
       </c>
       <c r="B954" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="955" spans="1:8" x14ac:dyDescent="0.2">
@@ -14651,7 +14696,7 @@
     </row>
     <row r="959" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A959" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B959">
         <v>-1</v>
@@ -14666,10 +14711,10 @@
         <v>13</v>
       </c>
       <c r="G959" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H959" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="960" spans="1:8" x14ac:dyDescent="0.2">
@@ -14764,7 +14809,7 @@
         <v>0</v>
       </c>
       <c r="B966" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="967" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -14796,7 +14841,7 @@
         <v>5</v>
       </c>
       <c r="B970" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="971" spans="1:8" x14ac:dyDescent="0.2">
@@ -14855,7 +14900,7 @@
     </row>
     <row r="975" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A975" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B975">
         <v>-1</v>
@@ -14870,10 +14915,10 @@
         <v>13</v>
       </c>
       <c r="G975" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H975" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="976" spans="1:8" x14ac:dyDescent="0.2">
@@ -15001,7 +15046,7 @@
     </row>
     <row r="982" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A982" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B982">
         <v>-0.46</v>
@@ -15016,7 +15061,7 @@
         <v>15</v>
       </c>
       <c r="G982" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="984" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -15034,7 +15079,7 @@
         <v>0</v>
       </c>
       <c r="B985" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C985" s="22"/>
       <c r="D985" s="22"/>
@@ -15098,7 +15143,7 @@
         <v>5</v>
       </c>
       <c r="B989" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C989" s="15"/>
       <c r="D989" s="15"/>
@@ -15185,7 +15230,7 @@
     </row>
     <row r="994" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A994" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B994" s="15">
         <v>-1</v>
@@ -15201,10 +15246,10 @@
         <v>13</v>
       </c>
       <c r="G994" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H994" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I994" s="15"/>
       <c r="J994" s="15"/>
@@ -15278,7 +15323,7 @@
         <v>264</v>
       </c>
       <c r="H997" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I997" s="15"/>
       <c r="J997" s="15"/>

</xml_diff>

<commit_message>
Reduce methyl chloride emission from Li-S battery manufacture from 1% to 0.5%.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-LiS.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-LiS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA59D2-4254-5241-BA6C-F264677CD2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41DEF73-0BD7-DE4D-9CBD-9EB9FFE2BF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31560" yWindow="-860" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1571,9 +1571,6 @@
     <t>This is a multi-output process, which produces dimethylchlorosilane (97%) but also trimethylchlorosilane (3%). The ecoinvent dataset for trimethylchlorosilane has been re-allocated to produce a proxy for dimethylchlorosilane production, based on a mass allocation. Note that, compared to the oroginal values in ecoinvent and also Wickerts et al., 2023, we have reduced the emission of methyl chloride, a potent ozone-depleting gas, to 1%, instead of 4.5%, which seems to ignore current efforts in limiting venting of such gases and promoting recovery instead. According to this report (https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf), the current leak rate in the EU is about 0.06%. Source: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141</t>
   </si>
   <si>
-    <t>Original value in Wickerts et al., 2023 of 0.0412, representing a 4.5% leakage rate. This was reduced to 1% leakage rate. According to https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf, current leakage rate in the EU is 0.06%.</t>
-  </si>
-  <si>
     <t>uncertainty type</t>
   </si>
   <si>
@@ -1584,6 +1581,9 @@
   </si>
   <si>
     <t>maximum</t>
+  </si>
+  <si>
+    <t>Original value in Wickerts et al., 2023 of 0.0412, representing a 4.5% leakage rate. This was reduced to 0.5% leakage rate. According to https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf, current leakage rate in the EU is 0.06%.</t>
   </si>
 </sst>
 </file>
@@ -1760,7 +1760,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1790,7 +1790,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2076,7 +2075,7 @@
   <dimension ref="A1:Q1076"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2935,7 +2934,7 @@
       <c r="A68" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="B68" t="s">
         <v>458</v>
       </c>
     </row>
@@ -3010,16 +3009,16 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
+        <v>459</v>
+      </c>
+      <c r="J75" t="s">
         <v>460</v>
       </c>
-      <c r="J75" t="s">
+      <c r="K75" t="s">
         <v>461</v>
       </c>
-      <c r="K75" t="s">
+      <c r="L75" t="s">
         <v>462</v>
-      </c>
-      <c r="L75" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
@@ -3416,8 +3415,8 @@
         <v>400</v>
       </c>
       <c r="B95" s="13">
-        <f>0.01*SUM(B82:B83)</f>
-        <v>8.2594999999999995E-3</v>
+        <f>0.005*SUM(B82:B83)</f>
+        <v>4.1297499999999997E-3</v>
       </c>
       <c r="C95" t="s">
         <v>7</v>
@@ -3429,18 +3428,18 @@
         <v>44</v>
       </c>
       <c r="H95" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="I95">
         <v>5</v>
       </c>
       <c r="J95" s="13">
         <f>B95</f>
-        <v>8.2594999999999995E-3</v>
+        <v>4.1297499999999997E-3</v>
       </c>
       <c r="K95">
-        <f>0.006*SUM(B82:B83)</f>
-        <v>4.9556999999999995E-3</v>
+        <f>0.0006*SUM(B82:B83)</f>
+        <v>4.9556999999999997E-4</v>
       </c>
       <c r="L95">
         <v>4.1300000000000003E-2</v>

</xml_diff>

<commit_message>
Updated metadata for methyltrichlorosilane production
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-LiS.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-LiS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41DEF73-0BD7-DE4D-9CBD-9EB9FFE2BF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ADDE62-F391-1E48-B22D-C70267C828F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="-860" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - Li-S" sheetId="1" r:id="rId1"/>
@@ -1568,9 +1568,6 @@
     <t>battery, Li-S</t>
   </si>
   <si>
-    <t>This is a multi-output process, which produces dimethylchlorosilane (97%) but also trimethylchlorosilane (3%). The ecoinvent dataset for trimethylchlorosilane has been re-allocated to produce a proxy for dimethylchlorosilane production, based on a mass allocation. Note that, compared to the oroginal values in ecoinvent and also Wickerts et al., 2023, we have reduced the emission of methyl chloride, a potent ozone-depleting gas, to 1%, instead of 4.5%, which seems to ignore current efforts in limiting venting of such gases and promoting recovery instead. According to this report (https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf), the current leak rate in the EU is about 0.06%. Source: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141</t>
-  </si>
-  <si>
     <t>uncertainty type</t>
   </si>
   <si>
@@ -1584,6 +1581,9 @@
   </si>
   <si>
     <t>Original value in Wickerts et al., 2023 of 0.0412, representing a 4.5% leakage rate. This was reduced to 0.5% leakage rate. According to https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf, current leakage rate in the EU is 0.06%.</t>
+  </si>
+  <si>
+    <t>This is a multi-output process, which produces dimethylchlorosilane (97%) but also trimethylchlorosilane (3%). The ecoinvent dataset for trimethylchlorosilane has been re-allocated to produce a proxy for dimethylchlorosilane production, based on a mass allocation. Note that, compared to the original values in ecoinvent and also Wickerts et al., 2023, we have reduced the emission of methyl chloride, a potent ozone-depleting gas, to 0.5%, instead of 4.5%, with a min-max of 0.06%-4.1%, as it seems to ignore current efforts in limiting venting of such gases and promoting recovery instead. According to this report (https://www.chlorinated-solvents.eu/wp-content/uploads/2021/05/Dichloromethane-paper.pdf), the current leak rate in the EU is about 0.06%. Source for Li-S battery: Wickerts et al. (2023). Prospective Life Cycle Assessment of Lithium-Sulfur Batteries for Stationary Energy Storage. ACS Sustainable Chemistry &amp; Engineering. https://doi.org/10.1021/acssuschemeng.3c00141. Source for trimethylchlorosilane: https://pubs.acs.org/doi/10.1021/acssuschemeng.1c00376</t>
   </si>
 </sst>
 </file>
@@ -2074,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1076"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2935,7 +2935,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -3009,16 +3009,16 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
+        <v>458</v>
+      </c>
+      <c r="J75" t="s">
         <v>459</v>
       </c>
-      <c r="J75" t="s">
+      <c r="K75" t="s">
         <v>460</v>
       </c>
-      <c r="K75" t="s">
+      <c r="L75" t="s">
         <v>461</v>
-      </c>
-      <c r="L75" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
@@ -3428,7 +3428,7 @@
         <v>44</v>
       </c>
       <c r="H95" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I95">
         <v>5</v>

</xml_diff>